<commit_message>
Updates to include Okanogan EDT results (and other general updates)
</commit_message>
<xml_diff>
--- a/Data/Criteria_and_Scoring/Criteria_Okanogan_EDT_Scoring.xlsx
+++ b/Data/Criteria_and_Scoring/Criteria_Okanogan_EDT_Scoring.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ryan\Documents\GitHub\Prioritization_Step2_Data_R_Project\Data\Criteria_and_Scoring\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{988999AF-01CF-4066-8C75-1E3F789B782A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3345D38C-650E-4F5F-AFF5-09C7E5849E09}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9264" yWindow="228" windowWidth="13740" windowHeight="11508" xr2:uid="{87D052C3-1649-48C9-991C-E0F89458B4FA}"/>
+    <workbookView xWindow="2988" yWindow="1548" windowWidth="17328" windowHeight="11508" xr2:uid="{87D052C3-1649-48C9-991C-E0F89458B4FA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="19">
   <si>
     <t>Condition</t>
   </si>
@@ -84,7 +84,13 @@
     <t>Level 3 Life Stage Performance Effect Scoring</t>
   </si>
   <si>
-    <t>Performance effect scores of 0 are ranked 5</t>
+    <t>Performance effect scores of 0 are ranked 5, oroginally ony had upper at 0.1, but multiple were above 0.1</t>
+  </si>
+  <si>
+    <t>for Performance Effect scores</t>
+  </si>
+  <si>
+    <t>for factorWeight scores</t>
   </si>
 </sst>
 </file>
@@ -454,7 +460,7 @@
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -515,6 +521,9 @@
       <c r="G2">
         <v>1</v>
       </c>
+      <c r="H2" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -538,6 +547,9 @@
       <c r="G3">
         <v>3</v>
       </c>
+      <c r="H3" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -561,6 +573,9 @@
       <c r="G4">
         <v>5</v>
       </c>
+      <c r="H4" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
@@ -584,6 +599,9 @@
       <c r="G5">
         <v>1</v>
       </c>
+      <c r="H5" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
@@ -607,6 +625,9 @@
       <c r="G6">
         <v>3</v>
       </c>
+      <c r="H6" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
@@ -630,6 +651,9 @@
       <c r="G7">
         <v>5</v>
       </c>
+      <c r="H7" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
@@ -653,6 +677,9 @@
       <c r="G8">
         <v>1</v>
       </c>
+      <c r="H8" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
@@ -676,6 +703,9 @@
       <c r="G9">
         <v>3</v>
       </c>
+      <c r="H9" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
@@ -694,7 +724,7 @@
         <v>-9.9999999999999995E-21</v>
       </c>
       <c r="F10">
-        <v>0.1</v>
+        <v>10</v>
       </c>
       <c r="G10">
         <v>5</v>

</xml_diff>

<commit_message>
Updates for Okanogan EDT, other misc updates
Updated Limiting Factor Pathway - to integrate EDT (Okanogan) results.

Also - integrated Okanogan (EDT) barrier results.
</commit_message>
<xml_diff>
--- a/Data/Criteria_and_Scoring/Criteria_Okanogan_EDT_Scoring.xlsx
+++ b/Data/Criteria_and_Scoring/Criteria_Okanogan_EDT_Scoring.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ryan\Documents\GitHub\Prioritization_Step2_Data_R_Project\Data\Criteria_and_Scoring\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3345D38C-650E-4F5F-AFF5-09C7E5849E09}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{053B3536-61A2-4D39-9F1F-E3AD0F69D2C8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2988" yWindow="1548" windowWidth="17328" windowHeight="11508" xr2:uid="{87D052C3-1649-48C9-991C-E0F89458B4FA}"/>
+    <workbookView xWindow="876" yWindow="660" windowWidth="20976" windowHeight="10572" xr2:uid="{87D052C3-1649-48C9-991C-E0F89458B4FA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$H$13</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -34,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="21">
   <si>
     <t>Condition</t>
   </si>
@@ -91,6 +94,12 @@
   </si>
   <si>
     <t>for factorWeight scores</t>
+  </si>
+  <si>
+    <t>for "Change in NEQ"</t>
+  </si>
+  <si>
+    <t>Level 3 Attribute - Obstructoins (Barrires)</t>
   </si>
 </sst>
 </file>
@@ -457,10 +466,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4190E53D-9721-4917-A41F-0C0211D2836D}">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -669,7 +678,7 @@
         <v>13</v>
       </c>
       <c r="E8">
-        <v>-1</v>
+        <v>-1.1000000000000001</v>
       </c>
       <c r="F8">
         <v>-0.01</v>
@@ -733,7 +742,86 @@
         <v>16</v>
       </c>
     </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11">
+        <v>1.2</v>
+      </c>
+      <c r="F11">
+        <v>10000</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="H11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" t="s">
+        <v>13</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>1.2</v>
+      </c>
+      <c r="G12">
+        <v>3</v>
+      </c>
+      <c r="H12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" t="s">
+        <v>12</v>
+      </c>
+      <c r="D13" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13">
+        <v>-10000</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>5</v>
+      </c>
+      <c r="H13" t="s">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
+  <autoFilter ref="A1:H13" xr:uid="{63F39076-0227-4BA7-AD8D-5B54291DE178}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>